<commit_message>
Small tweaks to method naming
</commit_message>
<xml_diff>
--- a/laptimey/vehicle/Steering and Kinematics/KinSheetUV19.xlsx
+++ b/laptimey/vehicle/Steering and Kinematics/KinSheetUV19.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F1AC4F-3722-4B17-9410-4252C5676E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A1057D-CFB5-41BA-80F6-D2371CB359D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="2496" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20892" yWindow="3108" windowWidth="17280" windowHeight="9108" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="delta" sheetId="6" r:id="rId1"/>
@@ -2236,7 +2236,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:J19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added surface fitting and useful tools
</commit_message>
<xml_diff>
--- a/laptimey/vehicle/Steering and Kinematics/KinSheetUV19.xlsx
+++ b/laptimey/vehicle/Steering and Kinematics/KinSheetUV19.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A1057D-CFB5-41BA-80F6-D2371CB359D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36E0D08-7D81-4432-B73E-A58E772D0C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20892" yWindow="3108" windowWidth="17280" windowHeight="9108" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31935" yWindow="6705" windowWidth="13830" windowHeight="7290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="delta" sheetId="6" r:id="rId1"/>
@@ -24,6 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Rack Travel [mm]</t>
   </si>
@@ -46,9 +50,6 @@
   </si>
   <si>
     <t>Bump Travel [mm]</t>
-  </si>
-  <si>
-    <t>Bump Travel [mm] \ Rack Travel [mm]</t>
   </si>
   <si>
     <t>Roll Angle [deg]</t>
@@ -105,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -122,6 +123,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,14 +681,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:V45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -757,61 +761,61 @@
       <c r="A2" s="1">
         <v>-30</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="10">
         <v>4.0170002</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="10">
         <v>3.6089999700000002</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="10">
         <v>3.1570000600000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="10">
         <v>2.8650000100000002</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="10">
         <v>2.5230000000000001</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="10">
         <v>2.2939999100000001</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="10">
         <v>2.0190000499999998</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="10">
         <v>1.8329999400000001</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="10">
         <v>1.6089999699999999</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="10">
         <v>1.4559999699999999</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="10">
         <v>1.31599998</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="10">
         <v>1.14699996</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="10">
         <v>1.03400004</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="10">
         <v>0.898999989</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="10">
         <v>0.80900001499999996</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="10">
         <v>0.70599997000000003</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="10">
         <v>0.63899999900000004</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="10">
         <v>0.56599998500000004</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="10">
         <v>0.52300000199999996</v>
       </c>
       <c r="U2" s="5"/>
@@ -820,61 +824,61 @@
       <c r="A3" s="1">
         <v>-27</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>3.9010000200000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>3.48799992</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>3.0309998999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <v>2.7360000599999998</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="10">
         <v>2.3900001</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="10">
         <v>2.16000009</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="10">
         <v>1.88399994</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="10">
         <v>1.6970000300000001</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="10">
         <v>1.472</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="10">
         <v>1.32000005</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="10">
         <v>1.17999995</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="10">
         <v>1.01199996</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="10">
         <v>0.898999989</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="10">
         <v>0.765999973</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="10">
         <v>0.676999986</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="10">
         <v>0.575999975</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="10">
         <v>0.512000024</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="10">
         <v>0.44100001500000002</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="10">
         <v>0.40000000600000002</v>
       </c>
       <c r="U3" s="5"/>
@@ -883,61 +887,61 @@
       <c r="A4" s="1">
         <v>-24</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>3.7839999199999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>3.3650000100000002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="10">
         <v>2.90199995</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="10">
         <v>2.60400009</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="10">
         <v>2.25600004</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="10">
         <v>2.02399993</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="10">
         <v>1.7460000499999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="10">
         <v>1.55900002</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="10">
         <v>1.3339999899999999</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="10">
         <v>1.1809999900000001</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="10">
         <v>1.0420000599999999</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="10">
         <v>0.875</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="10">
         <v>0.76300001100000003</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="10">
         <v>0.63099998199999996</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="10">
         <v>0.54400002999999997</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="10">
         <v>0.44499999299999998</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="10">
         <v>0.38199999899999998</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="10">
         <v>0.314999998</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="10">
         <v>0.275999993</v>
       </c>
       <c r="U4" s="5"/>
@@ -946,61 +950,61 @@
       <c r="A5" s="1">
         <v>-21</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>3.66400003</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>3.2400000100000002</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="10">
         <v>2.7720000699999998</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="10">
         <v>2.4709999599999999</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="10">
         <v>2.1199998899999999</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="10">
         <v>1.8860000400000001</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="10">
         <v>1.60699999</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="10">
         <v>1.4190000300000001</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="10">
         <v>1.1929999600000001</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="10">
         <v>1.0410000100000001</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="10">
         <v>0.90100002300000004</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="10">
         <v>0.73500001400000003</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="10">
         <v>0.62400001299999996</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="10">
         <v>0.493999988</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="10">
         <v>0.40799999199999998</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="10">
         <v>0.31099999</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="10">
         <v>0.25099998699999998</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="10">
         <v>0.186000004</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="10">
         <v>0.15000000599999999</v>
       </c>
       <c r="U5" s="5"/>
@@ -1009,61 +1013,61 @@
       <c r="A6" s="1">
         <v>-17</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="10">
         <v>3.5009999299999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="10">
         <v>3.0699999299999998</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="10">
         <v>2.59500003</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="10">
         <v>2.2899999599999998</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="10">
         <v>1.93499994</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="10">
         <v>1.6990000000000001</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="10">
         <v>1.41799998</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="10">
         <v>1.2289999700000001</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="10">
         <v>1.00300002</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="10">
         <v>0.85000002399999997</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="10">
         <v>0.71100002500000004</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="10">
         <v>0.54600000400000004</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="10">
         <v>0.43599999</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="10">
         <v>0.307999998</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="10">
         <v>0.22499999400000001</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="10">
         <v>0.12999999500000001</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="10">
         <v>7.1999996900000002E-2</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="10">
         <v>1.20000001E-2</v>
       </c>
-      <c r="T6" s="8">
+      <c r="T6" s="10">
         <v>-2.0999999700000001E-2</v>
       </c>
       <c r="U6" s="5"/>
@@ -1072,61 +1076,61 @@
       <c r="A7" s="1">
         <v>-14</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="10">
         <v>3.3770000900000001</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="10">
         <v>2.94000006</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="10">
         <v>2.4600000400000002</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="10">
         <v>2.15199995</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="10">
         <v>1.7940000300000001</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="10">
         <v>1.5559999900000001</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="10">
         <v>1.2740000499999999</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="10">
         <v>1.0839999899999999</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="10">
         <v>0.85799998</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="10">
         <v>0.704999983</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="10">
         <v>0.56699997199999996</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="10">
         <v>0.40200001000000002</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="10">
         <v>0.293000013</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="10">
         <v>0.16599999400000001</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="10">
         <v>8.3999998899999997E-2</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7" s="10">
         <v>-7.0000002200000001E-3</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7" s="10">
         <v>-6.3000001E-2</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="10">
         <v>-0.120999999</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="10">
         <v>-0.150999993</v>
       </c>
       <c r="U7" s="5"/>
@@ -1135,61 +1139,61 @@
       <c r="A8" s="1">
         <v>-11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="10">
         <v>3.25</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="10">
         <v>2.8080000900000002</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="10">
         <v>2.3220000299999999</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="10">
         <v>2.01200008</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="10">
         <v>1.6510000199999999</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="10">
         <v>1.4119999400000001</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="10">
         <v>1.12800002</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="10">
         <v>0.93699997700000004</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="10">
         <v>0.709999979</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="10">
         <v>0.55800002800000004</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="10">
         <v>0.41999998700000002</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="10">
         <v>0.256000012</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="10">
         <v>0.14800000199999999</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="10">
         <v>2.3E-2</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="10">
         <v>-5.7999998300000001E-2</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="10">
         <v>-0.14699999999999999</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="10">
         <v>-0.20100000500000001</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="10">
         <v>-0.256000012</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="10">
         <v>-0.28299999199999998</v>
       </c>
       <c r="U8" s="5"/>
@@ -1198,61 +1202,61 @@
       <c r="A9" s="1">
         <v>-8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="10">
         <v>3.1210000500000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="10">
         <v>2.6740000199999998</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="10">
         <v>2.1830000900000002</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="10">
         <v>1.86899996</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="10">
         <v>1.5049999999999999</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="10">
         <v>1.26499999</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="10">
         <v>0.978999972</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="10">
         <v>0.78799998800000004</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="10">
         <v>0.56099999</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="10">
         <v>0.409000009</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="10">
         <v>0.27099999800000002</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="10">
         <v>0.108000003</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="10">
         <v>1.00000005E-3</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="10">
         <v>-0.123000003</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="10">
         <v>-0.20200000700000001</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="10">
         <v>-0.289000005</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="10">
         <v>-0.340999991</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="10">
         <v>-0.39199999000000002</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="10">
         <v>-0.41699999599999998</v>
       </c>
       <c r="U9" s="5"/>
@@ -1261,61 +1265,61 @@
       <c r="A10" s="1">
         <v>-5</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="10">
         <v>2.9900000100000002</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <v>2.5369999399999998</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="10">
         <v>2.0409998900000001</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="10">
         <v>1.72500002</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="10">
         <v>1.3580000400000001</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="10">
         <v>1.11600006</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="10">
         <v>0.82899999599999996</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="10">
         <v>0.637000024</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="10">
         <v>0.409000009</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="10">
         <v>0.25699999899999998</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="10">
         <v>0.119999997</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="10">
         <v>-4.1999999400000002E-2</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="10">
         <v>-0.14800000199999999</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="10">
         <v>-0.27000001099999998</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="10">
         <v>-0.34799998999999998</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="10">
         <v>-0.432999998</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="10">
         <v>-0.48300000999999998</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="10">
         <v>-0.53100001799999996</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="10">
         <v>-0.55400002000000004</v>
       </c>
       <c r="U10" s="5"/>
@@ -1324,61 +1328,61 @@
       <c r="A11" s="1">
         <v>-2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="10">
         <v>2.85700011</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="10">
         <v>2.39899993</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="10">
         <v>1.89699996</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="10">
         <v>1.5779999499999999</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="10">
         <v>1.2079999400000001</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="10">
         <v>0.963999987</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="10">
         <v>0.67599999899999996</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="10">
         <v>0.48399999700000002</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="10">
         <v>0.256000012</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="10">
         <v>0.10400000199999999</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="10">
         <v>-3.4000001799999999E-2</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="10">
         <v>-0.194000006</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="10">
         <v>-0.30000001199999998</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="10">
         <v>-0.41999998700000002</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="10">
         <v>-0.495999992</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="10">
         <v>-0.57800000900000004</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="10">
         <v>-0.62599998700000004</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="10">
         <v>-0.67199999099999996</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="10">
         <v>-0.69199997199999996</v>
       </c>
       <c r="U11" s="5"/>
@@ -1387,61 +1391,61 @@
       <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="10">
         <v>2.6749999500000001</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="10">
         <v>2.2100000400000002</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="10">
         <v>1.7020000200000001</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="10">
         <v>1.3789999500000001</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="10">
         <v>1.0049999999999999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="10">
         <v>0.75900000300000003</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="10">
         <v>0.46900001200000002</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="10">
         <v>0.275999993</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="10">
         <v>4.69999984E-2</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="10">
         <v>-0.104999997</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="10">
         <v>-0.24099999699999999</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="10">
         <v>-0.400999993</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="10">
         <v>-0.50499999500000003</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="10">
         <v>-0.62300002600000004</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="10">
         <v>-0.69700002699999997</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="10">
         <v>-0.77600002300000004</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="10">
         <v>-0.82099997999999996</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="10">
         <v>-0.86199998899999997</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="10">
         <v>-0.879000008</v>
       </c>
       <c r="U12" s="5"/>
@@ -1450,61 +1454,61 @@
       <c r="A13" s="1">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="10">
         <v>2.53600001</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="10">
         <v>2.06599998</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="10">
         <v>1.5529999699999999</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="10">
         <v>1.2270000000000001</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="10">
         <v>0.85000002399999997</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="10">
         <v>0.60299998499999996</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="10">
         <v>0.31099999</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="10">
         <v>0.11800000099999999</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="10">
         <v>-0.111000001</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="10">
         <v>-0.26300001099999998</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="10">
         <v>-0.398999989</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="10">
         <v>-0.55800002800000004</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="10">
         <v>-0.661000013</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="10">
         <v>-0.77700000999999996</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="10">
         <v>-0.85000002399999997</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="10">
         <v>-0.92599999899999996</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="10">
         <v>-0.96899998200000004</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="10">
         <v>-1.0080000200000001</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="10">
         <v>-1.0210000299999999</v>
       </c>
       <c r="U13" s="5"/>
@@ -1513,61 +1517,61 @@
       <c r="A14" s="1">
         <v>8</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="10">
         <v>2.3949999800000001</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="10">
         <v>1.9199999599999999</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="10">
         <v>1.40199995</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="10">
         <v>1.07299995</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="10">
         <v>0.69300001899999997</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="10">
         <v>0.444000006</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="10">
         <v>0.150999993</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="10">
         <v>-4.3000001500000003E-2</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="10">
         <v>-0.27200001499999998</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="10">
         <v>-0.42399999500000002</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="10">
         <v>-0.560000002</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="10">
         <v>-0.71700000799999997</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="10">
         <v>-0.819000006</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="10">
         <v>-0.93400001499999996</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="10">
         <v>-1.0049999999999999</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="10">
         <v>-1.079</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="10">
         <v>-1.1200000000000001</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="10">
         <v>-1.15499997</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="10">
         <v>-1.1660000100000001</v>
       </c>
       <c r="U14" s="5"/>
@@ -1576,61 +1580,61 @@
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="10">
         <v>2.2509999299999999</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="10">
         <v>1.7710000299999999</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="10">
         <v>1.24800003</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="10">
         <v>0.916000009</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="10">
         <v>0.53399997899999996</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="10">
         <v>0.28299999199999998</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="10">
         <v>-1.09999999E-2</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="10">
         <v>-0.20599999999999999</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="10">
         <v>-0.435000002</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="10">
         <v>-0.58700001199999996</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="10">
         <v>-0.722000003</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="10">
         <v>-0.879000008</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="10">
         <v>-0.980000019</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="10">
         <v>-1.0930000499999999</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="10">
         <v>-1.1619999400000001</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="10">
         <v>-1.2339999699999999</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="10">
         <v>-1.2729999999999999</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="10">
         <v>-1.3040000199999999</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="10">
         <v>-1.31299996</v>
       </c>
       <c r="U15" s="5"/>
@@ -1639,61 +1643,61 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="10">
         <v>2.1050000199999999</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="10">
         <v>1.62</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="10">
         <v>1.09099996</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="10">
         <v>0.75700002899999996</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="10">
         <v>0.37200000900000002</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="10">
         <v>0.119999997</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="10">
         <v>-0.17599999899999999</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="10">
         <v>-0.370999992</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="10">
         <v>-0.601000011</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="10">
         <v>-0.75199997399999996</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="10">
         <v>-0.887000024</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="10">
         <v>-1.04299998</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="10">
         <v>-1.14300001</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="10">
         <v>-1.2539999500000001</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="10">
         <v>-1.3209999800000001</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="10">
         <v>-1.3910000300000001</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="10">
         <v>-1.4279999699999999</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="10">
         <v>-1.4559999699999999</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="10">
         <v>-1.4620000099999999</v>
       </c>
       <c r="U16" s="5"/>
@@ -1702,61 +1706,61 @@
       <c r="A17" s="1">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="10">
         <v>1.9559999699999999</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="10">
         <v>1.46599996</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="10">
         <v>0.93300002800000004</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="10">
         <v>0.59500002900000004</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="10">
         <v>0.20800000399999999</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="10">
         <v>-4.6000000100000001E-2</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="10">
         <v>-0.342999995</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="10">
         <v>-0.53899997499999996</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="10">
         <v>-0.76899999399999996</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="10">
         <v>-0.920000017</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="10">
         <v>-1.0540000199999999</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="10">
         <v>-1.2089999899999999</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="10">
         <v>-1.30799997</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="10">
         <v>-1.4170000599999999</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="10">
         <v>-1.4830000400000001</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="10">
         <v>-1.5499999499999999</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="10">
         <v>-1.5839999899999999</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="10">
         <v>-1.61000001</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="10">
         <v>-1.61300004</v>
       </c>
       <c r="U17" s="5"/>
@@ -1765,61 +1769,61 @@
       <c r="A18" s="1">
         <v>21</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="10">
         <v>1.75300002</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="10">
         <v>1.25600004</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="10">
         <v>0.71700000799999997</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="10">
         <v>0.37599998699999998</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="10">
         <v>-1.4999999700000001E-2</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="10">
         <v>-0.27000001099999998</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="10">
         <v>-0.569000006</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="10">
         <v>-0.765999973</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="10">
         <v>-0.995999992</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="10">
         <v>-1.14699996</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="10">
         <v>-1.28100002</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="10">
         <v>-1.43400002</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="10">
         <v>-1.53100002</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="10">
         <v>-1.6380000100000001</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="10">
         <v>-1.7020000200000001</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="10">
         <v>-1.7660000300000001</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="10">
         <v>-1.7970000500000001</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="10">
         <v>-1.8179999600000001</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="10">
         <v>-1.8179999600000001</v>
       </c>
       <c r="U18" s="5"/>
@@ -1828,61 +1832,61 @@
       <c r="A19" s="1">
         <v>24</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="10">
         <v>1.597</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="10">
         <v>1.0959999600000001</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="10">
         <v>0.551999986</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="10">
         <v>0.20900000599999999</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="10">
         <v>-0.185000002</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="10">
         <v>-0.442000002</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="10">
         <v>-0.741999984</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="10">
         <v>-0.93900001</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="10">
         <v>-1.1690000300000001</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="10">
         <v>-1.32000005</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="10">
         <v>-1.4529999499999999</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="10">
         <v>-1.60599995</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="10">
         <v>-1.7020000200000001</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="10">
         <v>-1.8070000399999999</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="10">
         <v>-1.86899996</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="10">
         <v>-1.92999995</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="10">
         <v>-1.9589999899999999</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="10">
         <v>-1.9770000000000001</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="10">
         <v>-1.9739999800000001</v>
       </c>
       <c r="U19" s="5"/>
@@ -1891,61 +1895,61 @@
       <c r="A20" s="1">
         <v>27</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="10">
         <v>1.43900001</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="10">
         <v>0.93400001499999996</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="10">
         <v>0.38499999000000001</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="10">
         <v>3.9000000799999997E-2</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="10">
         <v>-0.35800000999999998</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="10">
         <v>-0.61599999699999997</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="10">
         <v>-0.91699999600000004</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="10">
         <v>-1.1139999599999999</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="10">
         <v>-1.34500003</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="10">
         <v>-1.4950000000000001</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="10">
         <v>-1.62800002</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="10">
         <v>-1.7790000399999999</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="10">
         <v>-1.87399995</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="10">
         <v>-1.97800004</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="10">
         <v>-2.03800011</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="10">
         <v>-2.0959999599999999</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="10">
         <v>-2.1240000700000001</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="10">
         <v>-2.1380000099999998</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="10">
         <v>-2.1319999699999999</v>
       </c>
       <c r="U20" s="5"/>
@@ -1954,61 +1958,61 @@
       <c r="A21" s="1">
         <v>30</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="10">
         <v>1.278</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="10">
         <v>0.76800000700000004</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="10">
         <v>0.21500000399999999</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="10">
         <v>-0.13300000100000001</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="10">
         <v>-0.53299999200000003</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="10">
         <v>-0.79199999600000004</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="10">
         <v>-1.09399998</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="10">
         <v>-1.2920000599999999</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="10">
         <v>-1.5229999999999999</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="10">
         <v>-1.6729999799999999</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="10">
         <v>-1.8059999900000001</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="10">
         <v>-1.9559999699999999</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="10">
         <v>-2.0499999500000001</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="10">
         <v>-2.1510000200000001</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="10">
         <v>-2.2100000400000002</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="10">
         <v>-2.2650001</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="10">
         <v>-2.2899999599999998</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="10">
         <v>-2.3010001199999999</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="10">
         <v>-2.2929999799999998</v>
       </c>
       <c r="U21" s="5"/>
@@ -2035,6 +2039,30 @@
       <c r="T22" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:T21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:T63">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2058,7 +2086,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2235,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830BA682-D624-4885-97C4-895021BB7B60}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,7 +2276,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1">
         <v>-31</v>
@@ -3612,7 +3640,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3800,10 +3828,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4151,10 +4179,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished current form of kinematic equations
Documentation still needed to be added, especially doc string for each method and class
</commit_message>
<xml_diff>
--- a/laptimey/vehicle/Steering and Kinematics/KinSheetUV19.xlsx
+++ b/laptimey/vehicle/Steering and Kinematics/KinSheetUV19.xlsx
@@ -3,18 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36E0D08-7D81-4432-B73E-A58E772D0C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8D264F-16BB-4E1B-BB50-591F5B83966D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31935" yWindow="6705" windowWidth="13830" windowHeight="7290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="delta" sheetId="6" r:id="rId1"/>
-    <sheet name="KCAMf" sheetId="1" r:id="rId2"/>
-    <sheet name="KCAMr" sheetId="2" r:id="rId3"/>
-    <sheet name="KTOEf" sheetId="3" r:id="rId4"/>
-    <sheet name="KTOEr" sheetId="4" r:id="rId5"/>
-    <sheet name="RCAMf" sheetId="5" r:id="rId6"/>
-    <sheet name="RCAMr" sheetId="8" r:id="rId7"/>
+    <sheet name="K_CAM_f" sheetId="1" r:id="rId1"/>
+    <sheet name="K_CAM_r" sheetId="2" r:id="rId2"/>
+    <sheet name="K_TOE_f" sheetId="3" r:id="rId3"/>
+    <sheet name="K_TOE_r" sheetId="4" r:id="rId4"/>
+    <sheet name="R_CAM_f" sheetId="5" r:id="rId5"/>
+    <sheet name="R_CAM_r" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
-  <si>
-    <t>Rack Travel [mm]</t>
-  </si>
-  <si>
-    <t>Right Wheel Angle [deg]</t>
-  </si>
-  <si>
-    <t>Left Wheel Angle [deg]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Bump Travel [mm]\ Rack Travel [mm]</t>
   </si>
@@ -106,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -119,7 +109,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -403,287 +392,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F3C972-EEED-455B-87F6-A47E0501DC1D}">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>-31</v>
-      </c>
-      <c r="B2">
-        <v>-34.2610016</v>
-      </c>
-      <c r="C2">
-        <v>-26.271999399999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>-28</v>
-      </c>
-      <c r="B3">
-        <v>-29.7129993</v>
-      </c>
-      <c r="C3">
-        <v>-23.766000699999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-24</v>
-      </c>
-      <c r="B4">
-        <v>-24.420999500000001</v>
-      </c>
-      <c r="C4">
-        <v>-20.4330006</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-21</v>
-      </c>
-      <c r="B5">
-        <v>-20.8309994</v>
-      </c>
-      <c r="C5">
-        <v>-17.934000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>-17</v>
-      </c>
-      <c r="B6">
-        <v>-16.391000699999999</v>
-      </c>
-      <c r="C6">
-        <v>-14.593000399999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>-14</v>
-      </c>
-      <c r="B7">
-        <v>-13.257</v>
-      </c>
-      <c r="C7">
-        <v>-12.074999800000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>-10</v>
-      </c>
-      <c r="B8">
-        <v>-9.2760000199999997</v>
-      </c>
-      <c r="C8">
-        <v>-8.6909999800000008</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>-7</v>
-      </c>
-      <c r="B9">
-        <v>-6.4070000599999997</v>
-      </c>
-      <c r="C9">
-        <v>-6.1240000700000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>-3</v>
-      </c>
-      <c r="B10">
-        <v>-2.7030000699999999</v>
-      </c>
-      <c r="C10">
-        <v>-2.65199995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>2.65199995</v>
-      </c>
-      <c r="C12">
-        <v>2.7030000699999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>6.1240000700000001</v>
-      </c>
-      <c r="C13">
-        <v>6.4070000599999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>8.6909999800000008</v>
-      </c>
-      <c r="C14">
-        <v>9.2760000199999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>12.074999800000001</v>
-      </c>
-      <c r="C15">
-        <v>13.257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>14.593000399999999</v>
-      </c>
-      <c r="C16">
-        <v>16.391000699999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>17.934000000000001</v>
-      </c>
-      <c r="C17">
-        <v>20.8309994</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>24</v>
-      </c>
-      <c r="B18">
-        <v>20.4330006</v>
-      </c>
-      <c r="C18">
-        <v>24.420999500000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>28</v>
-      </c>
-      <c r="B19">
-        <v>23.766000699999999</v>
-      </c>
-      <c r="C19">
-        <v>29.7129993</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>31</v>
-      </c>
-      <c r="B20">
-        <v>26.271999399999999</v>
-      </c>
-      <c r="C20">
-        <v>34.2610016</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25:V45"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22:T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>-31</v>
@@ -755,67 +469,67 @@
       <c r="T1" s="1">
         <v>31</v>
       </c>
-      <c r="U1" s="7"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>-30</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>4.0170002</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>3.6089999700000002</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>3.1570000600000001</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>2.8650000100000002</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>2.5230000000000001</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="9">
         <v>2.2939999100000001</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="9">
         <v>2.0190000499999998</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="9">
         <v>1.8329999400000001</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>1.6089999699999999</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="9">
         <v>1.4559999699999999</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="9">
         <v>1.31599998</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="9">
         <v>1.14699996</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="9">
         <v>1.03400004</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="9">
         <v>0.898999989</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="9">
         <v>0.80900001499999996</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="9">
         <v>0.70599997000000003</v>
       </c>
-      <c r="R2" s="10">
+      <c r="R2" s="9">
         <v>0.63899999900000004</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="9">
         <v>0.56599998500000004</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="9">
         <v>0.52300000199999996</v>
       </c>
       <c r="U2" s="5"/>
@@ -824,61 +538,61 @@
       <c r="A3" s="1">
         <v>-27</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>3.9010000200000001</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>3.48799992</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>3.0309998999999999</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>2.7360000599999998</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>2.3900001</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>2.16000009</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>1.88399994</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <v>1.6970000300000001</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="9">
         <v>1.472</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>1.32000005</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
         <v>1.17999995</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <v>1.01199996</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <v>0.898999989</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="9">
         <v>0.765999973</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="9">
         <v>0.676999986</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="9">
         <v>0.575999975</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="9">
         <v>0.512000024</v>
       </c>
-      <c r="S3" s="10">
+      <c r="S3" s="9">
         <v>0.44100001500000002</v>
       </c>
-      <c r="T3" s="10">
+      <c r="T3" s="9">
         <v>0.40000000600000002</v>
       </c>
       <c r="U3" s="5"/>
@@ -887,61 +601,61 @@
       <c r="A4" s="1">
         <v>-24</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>3.7839999199999999</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>3.3650000100000002</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>2.90199995</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>2.60400009</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>2.25600004</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>2.02399993</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>1.7460000499999999</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>1.55900002</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>1.3339999899999999</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>1.1809999900000001</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <v>1.0420000599999999</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>0.875</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <v>0.76300001100000003</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <v>0.63099998199999996</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="9">
         <v>0.54400002999999997</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="9">
         <v>0.44499999299999998</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="9">
         <v>0.38199999899999998</v>
       </c>
-      <c r="S4" s="10">
+      <c r="S4" s="9">
         <v>0.314999998</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="9">
         <v>0.275999993</v>
       </c>
       <c r="U4" s="5"/>
@@ -950,61 +664,61 @@
       <c r="A5" s="1">
         <v>-21</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>3.66400003</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>3.2400000100000002</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>2.7720000699999998</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>2.4709999599999999</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>2.1199998899999999</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>1.8860000400000001</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>1.60699999</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>1.4190000300000001</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>1.1929999600000001</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <v>1.0410000100000001</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="9">
         <v>0.90100002300000004</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <v>0.73500001400000003</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="9">
         <v>0.62400001299999996</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <v>0.493999988</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="9">
         <v>0.40799999199999998</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="9">
         <v>0.31099999</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="9">
         <v>0.25099998699999998</v>
       </c>
-      <c r="S5" s="10">
+      <c r="S5" s="9">
         <v>0.186000004</v>
       </c>
-      <c r="T5" s="10">
+      <c r="T5" s="9">
         <v>0.15000000599999999</v>
       </c>
       <c r="U5" s="5"/>
@@ -1013,61 +727,61 @@
       <c r="A6" s="1">
         <v>-17</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>3.5009999299999999</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>3.0699999299999998</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>2.59500003</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>2.2899999599999998</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>1.93499994</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>1.6990000000000001</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>1.41799998</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>1.2289999700000001</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>1.00300002</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>0.85000002399999997</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <v>0.71100002500000004</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <v>0.54600000400000004</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="9">
         <v>0.43599999</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>0.307999998</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="9">
         <v>0.22499999400000001</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="9">
         <v>0.12999999500000001</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="9">
         <v>7.1999996900000002E-2</v>
       </c>
-      <c r="S6" s="10">
+      <c r="S6" s="9">
         <v>1.20000001E-2</v>
       </c>
-      <c r="T6" s="10">
+      <c r="T6" s="9">
         <v>-2.0999999700000001E-2</v>
       </c>
       <c r="U6" s="5"/>
@@ -1076,61 +790,61 @@
       <c r="A7" s="1">
         <v>-14</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>3.3770000900000001</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>2.94000006</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>2.4600000400000002</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>2.15199995</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>1.7940000300000001</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>1.5559999900000001</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>1.2740000499999999</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>1.0839999899999999</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>0.85799998</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <v>0.704999983</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="9">
         <v>0.56699997199999996</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <v>0.40200001000000002</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="9">
         <v>0.293000013</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <v>0.16599999400000001</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="9">
         <v>8.3999998899999997E-2</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="9">
         <v>-7.0000002200000001E-3</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="9">
         <v>-6.3000001E-2</v>
       </c>
-      <c r="S7" s="10">
+      <c r="S7" s="9">
         <v>-0.120999999</v>
       </c>
-      <c r="T7" s="10">
+      <c r="T7" s="9">
         <v>-0.150999993</v>
       </c>
       <c r="U7" s="5"/>
@@ -1139,61 +853,61 @@
       <c r="A8" s="1">
         <v>-11</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>3.25</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>2.8080000900000002</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>2.3220000299999999</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>2.01200008</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>1.6510000199999999</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>1.4119999400000001</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <v>1.12800002</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>0.93699997700000004</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>0.709999979</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>0.55800002800000004</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="9">
         <v>0.41999998700000002</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <v>0.256000012</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="9">
         <v>0.14800000199999999</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <v>2.3E-2</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="9">
         <v>-5.7999998300000001E-2</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="9">
         <v>-0.14699999999999999</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="9">
         <v>-0.20100000500000001</v>
       </c>
-      <c r="S8" s="10">
+      <c r="S8" s="9">
         <v>-0.256000012</v>
       </c>
-      <c r="T8" s="10">
+      <c r="T8" s="9">
         <v>-0.28299999199999998</v>
       </c>
       <c r="U8" s="5"/>
@@ -1202,61 +916,61 @@
       <c r="A9" s="1">
         <v>-8</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>3.1210000500000001</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>2.6740000199999998</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>2.1830000900000002</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>1.86899996</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>1.5049999999999999</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>1.26499999</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>0.978999972</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>0.78799998800000004</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>0.56099999</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <v>0.409000009</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="9">
         <v>0.27099999800000002</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="9">
         <v>0.108000003</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="9">
         <v>1.00000005E-3</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9">
         <v>-0.123000003</v>
       </c>
-      <c r="P9" s="10">
+      <c r="P9" s="9">
         <v>-0.20200000700000001</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="9">
         <v>-0.289000005</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="9">
         <v>-0.340999991</v>
       </c>
-      <c r="S9" s="10">
+      <c r="S9" s="9">
         <v>-0.39199999000000002</v>
       </c>
-      <c r="T9" s="10">
+      <c r="T9" s="9">
         <v>-0.41699999599999998</v>
       </c>
       <c r="U9" s="5"/>
@@ -1265,61 +979,61 @@
       <c r="A10" s="1">
         <v>-5</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>2.9900000100000002</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>2.5369999399999998</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>2.0409998900000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>1.72500002</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>1.3580000400000001</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>1.11600006</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <v>0.82899999599999996</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>0.637000024</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>0.409000009</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <v>0.25699999899999998</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <v>0.119999997</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>-4.1999999400000002E-2</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="9">
         <v>-0.14800000199999999</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <v>-0.27000001099999998</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="9">
         <v>-0.34799998999999998</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="9">
         <v>-0.432999998</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="9">
         <v>-0.48300000999999998</v>
       </c>
-      <c r="S10" s="10">
+      <c r="S10" s="9">
         <v>-0.53100001799999996</v>
       </c>
-      <c r="T10" s="10">
+      <c r="T10" s="9">
         <v>-0.55400002000000004</v>
       </c>
       <c r="U10" s="5"/>
@@ -1328,61 +1042,61 @@
       <c r="A11" s="1">
         <v>-2</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>2.85700011</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>2.39899993</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>1.89699996</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>1.5779999499999999</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>1.2079999400000001</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>0.963999987</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>0.67599999899999996</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>0.48399999700000002</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>0.256000012</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>0.10400000199999999</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="9">
         <v>-3.4000001799999999E-2</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>-0.194000006</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="9">
         <v>-0.30000001199999998</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>-0.41999998700000002</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11" s="9">
         <v>-0.495999992</v>
       </c>
-      <c r="Q11" s="10">
+      <c r="Q11" s="9">
         <v>-0.57800000900000004</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R11" s="9">
         <v>-0.62599998700000004</v>
       </c>
-      <c r="S11" s="10">
+      <c r="S11" s="9">
         <v>-0.67199999099999996</v>
       </c>
-      <c r="T11" s="10">
+      <c r="T11" s="9">
         <v>-0.69199997199999996</v>
       </c>
       <c r="U11" s="5"/>
@@ -1391,61 +1105,61 @@
       <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>2.6749999500000001</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>2.2100000400000002</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>1.7020000200000001</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>1.3789999500000001</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>1.0049999999999999</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>0.75900000300000003</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <v>0.46900001200000002</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>0.275999993</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>4.69999984E-2</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>-0.104999997</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="9">
         <v>-0.24099999699999999</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="9">
         <v>-0.400999993</v>
       </c>
-      <c r="N12" s="10">
+      <c r="N12" s="9">
         <v>-0.50499999500000003</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9">
         <v>-0.62300002600000004</v>
       </c>
-      <c r="P12" s="10">
+      <c r="P12" s="9">
         <v>-0.69700002699999997</v>
       </c>
-      <c r="Q12" s="10">
+      <c r="Q12" s="9">
         <v>-0.77600002300000004</v>
       </c>
-      <c r="R12" s="10">
+      <c r="R12" s="9">
         <v>-0.82099997999999996</v>
       </c>
-      <c r="S12" s="10">
+      <c r="S12" s="9">
         <v>-0.86199998899999997</v>
       </c>
-      <c r="T12" s="10">
+      <c r="T12" s="9">
         <v>-0.879000008</v>
       </c>
       <c r="U12" s="5"/>
@@ -1454,61 +1168,61 @@
       <c r="A13" s="1">
         <v>5</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>2.53600001</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>2.06599998</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>1.5529999699999999</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>1.2270000000000001</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>0.85000002399999997</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>0.60299998499999996</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <v>0.31099999</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>0.11800000099999999</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>-0.111000001</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>-0.26300001099999998</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="9">
         <v>-0.398999989</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="9">
         <v>-0.55800002800000004</v>
       </c>
-      <c r="N13" s="10">
+      <c r="N13" s="9">
         <v>-0.661000013</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <v>-0.77700000999999996</v>
       </c>
-      <c r="P13" s="10">
+      <c r="P13" s="9">
         <v>-0.85000002399999997</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="Q13" s="9">
         <v>-0.92599999899999996</v>
       </c>
-      <c r="R13" s="10">
+      <c r="R13" s="9">
         <v>-0.96899998200000004</v>
       </c>
-      <c r="S13" s="10">
+      <c r="S13" s="9">
         <v>-1.0080000200000001</v>
       </c>
-      <c r="T13" s="10">
+      <c r="T13" s="9">
         <v>-1.0210000299999999</v>
       </c>
       <c r="U13" s="5"/>
@@ -1517,61 +1231,61 @@
       <c r="A14" s="1">
         <v>8</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>2.3949999800000001</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>1.9199999599999999</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>1.40199995</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>1.07299995</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>0.69300001899999997</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>0.444000006</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>0.150999993</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>-4.3000001500000003E-2</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>-0.27200001499999998</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <v>-0.42399999500000002</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9">
         <v>-0.560000002</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="9">
         <v>-0.71700000799999997</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="9">
         <v>-0.819000006</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>-0.93400001499999996</v>
       </c>
-      <c r="P14" s="10">
+      <c r="P14" s="9">
         <v>-1.0049999999999999</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="Q14" s="9">
         <v>-1.079</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="9">
         <v>-1.1200000000000001</v>
       </c>
-      <c r="S14" s="10">
+      <c r="S14" s="9">
         <v>-1.15499997</v>
       </c>
-      <c r="T14" s="10">
+      <c r="T14" s="9">
         <v>-1.1660000100000001</v>
       </c>
       <c r="U14" s="5"/>
@@ -1580,61 +1294,61 @@
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>2.2509999299999999</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>1.7710000299999999</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>1.24800003</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>0.916000009</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>0.53399997899999996</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>0.28299999199999998</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="9">
         <v>-1.09999999E-2</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="9">
         <v>-0.20599999999999999</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <v>-0.435000002</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="9">
         <v>-0.58700001199999996</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="9">
         <v>-0.722000003</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="9">
         <v>-0.879000008</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="9">
         <v>-0.980000019</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="9">
         <v>-1.0930000499999999</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="9">
         <v>-1.1619999400000001</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="9">
         <v>-1.2339999699999999</v>
       </c>
-      <c r="R15" s="10">
+      <c r="R15" s="9">
         <v>-1.2729999999999999</v>
       </c>
-      <c r="S15" s="10">
+      <c r="S15" s="9">
         <v>-1.3040000199999999</v>
       </c>
-      <c r="T15" s="10">
+      <c r="T15" s="9">
         <v>-1.31299996</v>
       </c>
       <c r="U15" s="5"/>
@@ -1643,61 +1357,61 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>2.1050000199999999</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>1.62</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>1.09099996</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>0.75700002899999996</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>0.37200000900000002</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="9">
         <v>0.119999997</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="9">
         <v>-0.17599999899999999</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="9">
         <v>-0.370999992</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="9">
         <v>-0.601000011</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="9">
         <v>-0.75199997399999996</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="9">
         <v>-0.887000024</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="9">
         <v>-1.04299998</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="9">
         <v>-1.14300001</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="9">
         <v>-1.2539999500000001</v>
       </c>
-      <c r="P16" s="10">
+      <c r="P16" s="9">
         <v>-1.3209999800000001</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="9">
         <v>-1.3910000300000001</v>
       </c>
-      <c r="R16" s="10">
+      <c r="R16" s="9">
         <v>-1.4279999699999999</v>
       </c>
-      <c r="S16" s="10">
+      <c r="S16" s="9">
         <v>-1.4559999699999999</v>
       </c>
-      <c r="T16" s="10">
+      <c r="T16" s="9">
         <v>-1.4620000099999999</v>
       </c>
       <c r="U16" s="5"/>
@@ -1706,61 +1420,61 @@
       <c r="A17" s="1">
         <v>17</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>1.9559999699999999</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>1.46599996</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>0.93300002800000004</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>0.59500002900000004</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>0.20800000399999999</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>-4.6000000100000001E-2</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="9">
         <v>-0.342999995</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>-0.53899997499999996</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9">
         <v>-0.76899999399999996</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="9">
         <v>-0.920000017</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="9">
         <v>-1.0540000199999999</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="9">
         <v>-1.2089999899999999</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="9">
         <v>-1.30799997</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="9">
         <v>-1.4170000599999999</v>
       </c>
-      <c r="P17" s="10">
+      <c r="P17" s="9">
         <v>-1.4830000400000001</v>
       </c>
-      <c r="Q17" s="10">
+      <c r="Q17" s="9">
         <v>-1.5499999499999999</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="9">
         <v>-1.5839999899999999</v>
       </c>
-      <c r="S17" s="10">
+      <c r="S17" s="9">
         <v>-1.61000001</v>
       </c>
-      <c r="T17" s="10">
+      <c r="T17" s="9">
         <v>-1.61300004</v>
       </c>
       <c r="U17" s="5"/>
@@ -1769,61 +1483,61 @@
       <c r="A18" s="1">
         <v>21</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>1.75300002</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>1.25600004</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>0.71700000799999997</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>0.37599998699999998</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <v>-1.4999999700000001E-2</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>-0.27000001099999998</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="9">
         <v>-0.569000006</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="9">
         <v>-0.765999973</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="9">
         <v>-0.995999992</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <v>-1.14699996</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="9">
         <v>-1.28100002</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="9">
         <v>-1.43400002</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="9">
         <v>-1.53100002</v>
       </c>
-      <c r="O18" s="10">
+      <c r="O18" s="9">
         <v>-1.6380000100000001</v>
       </c>
-      <c r="P18" s="10">
+      <c r="P18" s="9">
         <v>-1.7020000200000001</v>
       </c>
-      <c r="Q18" s="10">
+      <c r="Q18" s="9">
         <v>-1.7660000300000001</v>
       </c>
-      <c r="R18" s="10">
+      <c r="R18" s="9">
         <v>-1.7970000500000001</v>
       </c>
-      <c r="S18" s="10">
+      <c r="S18" s="9">
         <v>-1.8179999600000001</v>
       </c>
-      <c r="T18" s="10">
+      <c r="T18" s="9">
         <v>-1.8179999600000001</v>
       </c>
       <c r="U18" s="5"/>
@@ -1832,61 +1546,61 @@
       <c r="A19" s="1">
         <v>24</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>1.597</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>1.0959999600000001</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>0.551999986</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>0.20900000599999999</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <v>-0.185000002</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <v>-0.442000002</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="9">
         <v>-0.741999984</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="9">
         <v>-0.93900001</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="9">
         <v>-1.1690000300000001</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>-1.32000005</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="9">
         <v>-1.4529999499999999</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="9">
         <v>-1.60599995</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="9">
         <v>-1.7020000200000001</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="9">
         <v>-1.8070000399999999</v>
       </c>
-      <c r="P19" s="10">
+      <c r="P19" s="9">
         <v>-1.86899996</v>
       </c>
-      <c r="Q19" s="10">
+      <c r="Q19" s="9">
         <v>-1.92999995</v>
       </c>
-      <c r="R19" s="10">
+      <c r="R19" s="9">
         <v>-1.9589999899999999</v>
       </c>
-      <c r="S19" s="10">
+      <c r="S19" s="9">
         <v>-1.9770000000000001</v>
       </c>
-      <c r="T19" s="10">
+      <c r="T19" s="9">
         <v>-1.9739999800000001</v>
       </c>
       <c r="U19" s="5"/>
@@ -1895,61 +1609,61 @@
       <c r="A20" s="1">
         <v>27</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>1.43900001</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>0.93400001499999996</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>0.38499999000000001</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>3.9000000799999997E-2</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>-0.35800000999999998</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>-0.61599999699999997</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="9">
         <v>-0.91699999600000004</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>-1.1139999599999999</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="9">
         <v>-1.34500003</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>-1.4950000000000001</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="9">
         <v>-1.62800002</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>-1.7790000399999999</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="9">
         <v>-1.87399995</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9">
         <v>-1.97800004</v>
       </c>
-      <c r="P20" s="10">
+      <c r="P20" s="9">
         <v>-2.03800011</v>
       </c>
-      <c r="Q20" s="10">
+      <c r="Q20" s="9">
         <v>-2.0959999599999999</v>
       </c>
-      <c r="R20" s="10">
+      <c r="R20" s="9">
         <v>-2.1240000700000001</v>
       </c>
-      <c r="S20" s="10">
+      <c r="S20" s="9">
         <v>-2.1380000099999998</v>
       </c>
-      <c r="T20" s="10">
+      <c r="T20" s="9">
         <v>-2.1319999699999999</v>
       </c>
       <c r="U20" s="5"/>
@@ -1958,61 +1672,61 @@
       <c r="A21" s="1">
         <v>30</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>1.278</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>0.76800000700000004</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>0.21500000399999999</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>-0.13300000100000001</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>-0.53299999200000003</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>-0.79199999600000004</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="9">
         <v>-1.09399998</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="9">
         <v>-1.2920000599999999</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="9">
         <v>-1.5229999999999999</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="9">
         <v>-1.6729999799999999</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="9">
         <v>-1.8059999900000001</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="9">
         <v>-1.9559999699999999</v>
       </c>
-      <c r="N21" s="10">
+      <c r="N21" s="9">
         <v>-2.0499999500000001</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="9">
         <v>-2.1510000200000001</v>
       </c>
-      <c r="P21" s="10">
+      <c r="P21" s="9">
         <v>-2.2100000400000002</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="Q21" s="9">
         <v>-2.2650001</v>
       </c>
-      <c r="R21" s="10">
+      <c r="R21" s="9">
         <v>-2.2899999599999998</v>
       </c>
-      <c r="S21" s="10">
+      <c r="S21" s="9">
         <v>-2.3010001199999999</v>
       </c>
-      <c r="T21" s="10">
+      <c r="T21" s="9">
         <v>-2.2929999799999998</v>
       </c>
       <c r="U21" s="5"/>
@@ -2038,6 +1752,426 @@
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
     </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:T21">
     <cfRule type="colorScale" priority="2">
@@ -2051,7 +2185,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:T63">
+  <conditionalFormatting sqref="B43:T63">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2067,12 +2201,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A37F1D4-4DCF-4599-B42A-7B8FEA96519C}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,167 +2217,167 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>30</v>
+      <c r="A2" s="1">
+        <v>-30</v>
       </c>
       <c r="B2">
         <v>1.6390000600000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>27</v>
+      <c r="A3" s="1">
+        <v>-27</v>
       </c>
       <c r="B3">
         <v>1.4859999399999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>24</v>
+      <c r="A4" s="1">
+        <v>-24</v>
       </c>
       <c r="B4">
         <v>1.3309999699999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>21</v>
+      <c r="A5" s="1">
+        <v>-21</v>
       </c>
       <c r="B5">
         <v>1.1729999799999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>17</v>
+      <c r="A6" s="1">
+        <v>-17</v>
       </c>
       <c r="B6">
         <v>0.958999991</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>14</v>
+      <c r="A7" s="1">
+        <v>-14</v>
       </c>
       <c r="B7">
         <v>0.79600000400000004</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1">
+        <v>-11</v>
       </c>
       <c r="B8">
         <v>0.62999999500000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" s="1">
+        <v>-8</v>
       </c>
       <c r="B9">
         <v>0.46200001200000002</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
+      <c r="A10" s="1">
+        <v>-5</v>
       </c>
       <c r="B10">
         <v>0.291000009</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
+      <c r="A11" s="1">
+        <v>-2</v>
       </c>
       <c r="B11">
         <v>0.11699999899999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>-2</v>
+      <c r="A12" s="1">
+        <v>2</v>
       </c>
       <c r="B12">
         <v>-0.11800000099999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>-5</v>
+      <c r="A13" s="1">
+        <v>5</v>
       </c>
       <c r="B13">
         <v>-0.29800000799999998</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>-8</v>
+      <c r="A14" s="1">
+        <v>8</v>
       </c>
       <c r="B14">
         <v>-0.47999998900000002</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>-11</v>
+      <c r="A15" s="1">
+        <v>11</v>
       </c>
       <c r="B15">
         <v>-0.666000009</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>-14</v>
+      <c r="A16" s="1">
+        <v>14</v>
       </c>
       <c r="B16">
         <v>-0.853999972</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>-17</v>
+      <c r="A17" s="1">
+        <v>17</v>
       </c>
       <c r="B17">
         <v>-1.0440000300000001</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>-21</v>
+      <c r="A18" s="1">
+        <v>21</v>
       </c>
       <c r="B18">
         <v>-1.3029999699999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>-24</v>
+      <c r="A19" s="1">
+        <v>24</v>
       </c>
       <c r="B19">
         <v>-1.50100005</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>-27</v>
+      <c r="A20" s="1">
+        <v>27</v>
       </c>
       <c r="B20">
         <v>-1.70099998</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>-30</v>
+      <c r="A21" s="1">
+        <v>30</v>
       </c>
       <c r="B21">
         <v>-1.90499997</v>
@@ -2259,12 +2393,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830BA682-D624-4885-97C4-895021BB7B60}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,7 +2410,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>-31</v>
@@ -2335,7 +2469,7 @@
       <c r="T1" s="1">
         <v>31</v>
       </c>
-      <c r="U1" s="7"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -2368,7 +2502,7 @@
       <c r="J2">
         <v>-2.6380000099999998</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <v>8.2000002299999999E-2</v>
       </c>
       <c r="L2">
@@ -2431,7 +2565,7 @@
       <c r="J3">
         <v>-2.64899993</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <v>7.0000000300000004E-2</v>
       </c>
       <c r="L3">
@@ -2494,7 +2628,7 @@
       <c r="J4">
         <v>-2.6589999199999999</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="7">
         <v>5.9000000400000002E-2</v>
       </c>
       <c r="L4">
@@ -2557,7 +2691,7 @@
       <c r="J5">
         <v>-2.6670000599999999</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>4.8999998699999998E-2</v>
       </c>
       <c r="L5">
@@ -2620,7 +2754,7 @@
       <c r="J6">
         <v>-2.6779999700000001</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <v>3.5999998499999998E-2</v>
       </c>
       <c r="L6">
@@ -2683,7 +2817,7 @@
       <c r="J7">
         <v>-2.68499994</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>2.8000000899999999E-2</v>
       </c>
       <c r="L7">
@@ -2746,7 +2880,7 @@
       <c r="J8">
         <v>-2.69099998</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>1.9999999599999999E-2</v>
       </c>
       <c r="L8">
@@ -2809,7 +2943,7 @@
       <c r="J9">
         <v>-2.6949999299999998</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>1.30000003E-2</v>
       </c>
       <c r="L9">
@@ -2872,7 +3006,7 @@
       <c r="J10">
         <v>-2.6989998800000001</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <v>8.0000003800000004E-3</v>
       </c>
       <c r="L10">
@@ -2935,7 +3069,7 @@
       <c r="J11">
         <v>-2.7019999000000001</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="7">
         <v>3.0000000299999999E-3</v>
       </c>
       <c r="L11">
@@ -2998,7 +3132,7 @@
       <c r="J12">
         <v>-2.7040000000000002</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <v>-2.0000000900000001E-3</v>
       </c>
       <c r="L12">
@@ -3061,7 +3195,7 @@
       <c r="J13">
         <v>-2.7049999200000001</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>-4.9999998899999997E-3</v>
       </c>
       <c r="L13">
@@ -3124,7 +3258,7 @@
       <c r="J14">
         <v>-2.7040000000000002</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <v>-7.0000002200000001E-3</v>
       </c>
       <c r="L14">
@@ -3187,7 +3321,7 @@
       <c r="J15">
         <v>-2.7019999000000001</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="7">
         <v>-8.0000003800000004E-3</v>
       </c>
       <c r="L15">
@@ -3250,7 +3384,7 @@
       <c r="J16">
         <v>-2.6989998800000001</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="7">
         <v>-8.0000003800000004E-3</v>
       </c>
       <c r="L16">
@@ -3313,7 +3447,7 @@
       <c r="J17">
         <v>-2.6949999299999998</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="7">
         <v>-6.0000000499999999E-3</v>
       </c>
       <c r="L17">
@@ -3376,7 +3510,7 @@
       <c r="J18">
         <v>-2.68799996</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="7">
         <v>-3.0000000299999999E-3</v>
       </c>
       <c r="L18">
@@ -3502,7 +3636,7 @@
       <c r="J20">
         <v>-2.6730000999999999</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="7">
         <v>4.9999998899999997E-3</v>
       </c>
       <c r="L20">
@@ -3565,7 +3699,7 @@
       <c r="J21">
         <v>-2.66300011</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="7">
         <v>1.09999999E-2</v>
       </c>
       <c r="L21">
@@ -3618,16 +3752,39 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F9D592-8E53-46DC-87F6-8C0B08A4D3E9}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3637,14 +3794,14 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>-30</v>
       </c>
       <c r="B2">
@@ -3652,7 +3809,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>-27</v>
       </c>
       <c r="B3">
@@ -3660,146 +3817,146 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>-24</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>-9.3000002200000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>-21</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>-7.8000001599999993E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>-17</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>-5.9000000400000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>-14</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>-4.69999984E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>-11</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>-3.5000000099999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>-8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>-2.40000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>-5</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>-1.40000004E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>-2</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>-4.9999998899999997E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>2</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>4.9999998899999997E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>5</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>1.20000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>8</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>1.7000000899999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>11</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>2.1999999900000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>2.6000000499999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="8">
         <v>17</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>2.8000000899999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>21</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>2.99999993E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>24</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>3.09999995E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <v>27</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>2.99999993E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <v>30</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>2.8000000899999999E-2</v>
       </c>
     </row>
@@ -3812,7 +3969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B6817A-17BD-4083-962C-EA5A882AFE85}">
   <dimension ref="A1:B42"/>
   <sheetViews>
@@ -3828,10 +3985,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3990,7 +4147,7 @@
       <c r="A21">
         <v>-0.112000003</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>5.0000000699999998E-2</v>
       </c>
     </row>
@@ -4006,7 +4163,7 @@
       <c r="A23">
         <v>0.112000003</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="7">
         <v>-5.0000000699999998E-2</v>
       </c>
     </row>
@@ -4167,11 +4324,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CF82B5-6E7B-453F-B54B-473BA8641EF8}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4179,10 +4336,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4333,7 +4490,7 @@
       <c r="A20">
         <v>-0.22499999400000001</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>8.9000001499999995E-2</v>
       </c>
     </row>
@@ -4341,7 +4498,7 @@
       <c r="A21">
         <v>-0.112000003</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>4.5000001800000002E-2</v>
       </c>
     </row>
@@ -4357,7 +4514,7 @@
       <c r="A23">
         <v>0.112000003</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="7">
         <v>-4.5000001800000002E-2</v>
       </c>
     </row>
@@ -4365,7 +4522,7 @@
       <c r="A24">
         <v>0.22499999400000001</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="7">
         <v>-9.0999998200000001E-2</v>
       </c>
     </row>

</xml_diff>